<commit_message>
#Peterson - Telas, Requisitos e Cronograma
</commit_message>
<xml_diff>
--- a/2018-04-02 a 2018-04-06 correlatos,RF,RNF,projeto telas e cronograma/Cronograma.xlsx
+++ b/2018-04-02 a 2018-04-06 correlatos,RF,RNF,projeto telas e cronograma/Cronograma.xlsx
@@ -102,7 +102,7 @@
     <t>Implantação</t>
   </si>
   <si>
-    <t xml:space="preserve">UC04 - </t>
+    <t>UC04 - Encontrar Imagens atravéz do mapa</t>
   </si>
 </sst>
 </file>
@@ -471,21 +471,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -519,6 +504,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -822,8 +822,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -834,30 +834,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="19" t="s">
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19" t="s">
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
-      <c r="O1" s="19"/>
-      <c r="P1" s="19" t="s">
+      <c r="M1" s="36"/>
+      <c r="N1" s="36"/>
+      <c r="O1" s="36"/>
+      <c r="P1" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="Q1" s="19"/>
-      <c r="R1" s="19"/>
-      <c r="S1" s="19"/>
+      <c r="Q1" s="36"/>
+      <c r="R1" s="36"/>
+      <c r="S1" s="36"/>
     </row>
     <row r="2" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D2" s="14" t="s">
@@ -920,22 +920,22 @@
       <c r="C3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="20"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="21"/>
-      <c r="J3" s="21"/>
-      <c r="K3" s="22"/>
-      <c r="L3" s="20"/>
-      <c r="M3" s="21"/>
-      <c r="N3" s="21"/>
-      <c r="O3" s="22"/>
-      <c r="P3" s="20"/>
-      <c r="Q3" s="21"/>
-      <c r="R3" s="21"/>
-      <c r="S3" s="22"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
+      <c r="K3" s="39"/>
+      <c r="L3" s="37"/>
+      <c r="M3" s="38"/>
+      <c r="N3" s="38"/>
+      <c r="O3" s="39"/>
+      <c r="P3" s="37"/>
+      <c r="Q3" s="38"/>
+      <c r="R3" s="38"/>
+      <c r="S3" s="39"/>
       <c r="T3" s="1"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
@@ -1174,226 +1174,226 @@
       <c r="S10" s="12"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" s="33"/>
+      <c r="A11" s="28"/>
       <c r="B11" s="5" t="s">
         <v>28</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="28"/>
-      <c r="E11" s="29"/>
-      <c r="F11" s="29"/>
-      <c r="G11" s="30"/>
-      <c r="H11" s="28"/>
-      <c r="I11" s="29"/>
-      <c r="J11" s="29"/>
-      <c r="K11" s="30"/>
-      <c r="L11" s="28"/>
-      <c r="M11" s="29"/>
-      <c r="N11" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="O11" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="P11" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q11" s="29"/>
-      <c r="R11" s="29"/>
-      <c r="S11" s="30"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="23"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="25"/>
+      <c r="L11" s="23"/>
+      <c r="M11" s="24"/>
+      <c r="N11" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="O11" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="P11" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q11" s="24"/>
+      <c r="R11" s="24"/>
+      <c r="S11" s="25"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12" s="24" t="s">
+      <c r="A12" s="19" t="s">
         <v>20</v>
       </c>
       <c r="B12" s="7"/>
       <c r="C12" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="25"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="I12" s="26"/>
-      <c r="J12" s="26"/>
-      <c r="K12" s="27"/>
-      <c r="L12" s="25"/>
-      <c r="M12" s="26"/>
-      <c r="N12" s="26"/>
-      <c r="O12" s="27"/>
-      <c r="P12" s="25"/>
-      <c r="Q12" s="26"/>
-      <c r="R12" s="26"/>
-      <c r="S12" s="27"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="I12" s="21"/>
+      <c r="J12" s="21"/>
+      <c r="K12" s="22"/>
+      <c r="L12" s="20"/>
+      <c r="M12" s="21"/>
+      <c r="N12" s="21"/>
+      <c r="O12" s="22"/>
+      <c r="P12" s="20"/>
+      <c r="Q12" s="21"/>
+      <c r="R12" s="21"/>
+      <c r="S12" s="22"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="34" t="s">
+      <c r="A13" s="29" t="s">
         <v>21</v>
       </c>
       <c r="B13" s="7"/>
       <c r="C13" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="25"/>
-      <c r="E13" s="26"/>
-      <c r="F13" s="26"/>
-      <c r="G13" s="27"/>
-      <c r="H13" s="25"/>
-      <c r="I13" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="J13" s="26"/>
-      <c r="K13" s="27"/>
-      <c r="L13" s="25"/>
-      <c r="M13" s="26"/>
-      <c r="N13" s="26"/>
-      <c r="O13" s="27"/>
-      <c r="P13" s="25"/>
-      <c r="Q13" s="26"/>
-      <c r="R13" s="26"/>
-      <c r="S13" s="27"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="J13" s="21"/>
+      <c r="K13" s="22"/>
+      <c r="L13" s="20"/>
+      <c r="M13" s="21"/>
+      <c r="N13" s="21"/>
+      <c r="O13" s="22"/>
+      <c r="P13" s="20"/>
+      <c r="Q13" s="21"/>
+      <c r="R13" s="21"/>
+      <c r="S13" s="22"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="34" t="s">
+      <c r="A14" s="29" t="s">
         <v>22</v>
       </c>
       <c r="B14" s="7"/>
       <c r="C14" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="25"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="25"/>
-      <c r="I14" s="26"/>
-      <c r="J14" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="K14" s="27"/>
-      <c r="L14" s="25"/>
-      <c r="M14" s="26"/>
-      <c r="N14" s="26"/>
-      <c r="O14" s="27"/>
-      <c r="P14" s="25"/>
-      <c r="Q14" s="26"/>
-      <c r="R14" s="26"/>
-      <c r="S14" s="27"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="K14" s="22"/>
+      <c r="L14" s="20"/>
+      <c r="M14" s="21"/>
+      <c r="N14" s="21"/>
+      <c r="O14" s="22"/>
+      <c r="P14" s="20"/>
+      <c r="Q14" s="21"/>
+      <c r="R14" s="21"/>
+      <c r="S14" s="22"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" s="34" t="s">
+      <c r="A15" s="29" t="s">
         <v>24</v>
       </c>
       <c r="B15" s="7"/>
       <c r="C15" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="25"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="27"/>
-      <c r="H15" s="25"/>
-      <c r="I15" s="26"/>
-      <c r="J15" s="26"/>
-      <c r="K15" s="27"/>
-      <c r="L15" s="25"/>
-      <c r="M15" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="N15" s="26"/>
-      <c r="O15" s="27"/>
-      <c r="P15" s="25"/>
-      <c r="Q15" s="26"/>
-      <c r="R15" s="26"/>
-      <c r="S15" s="27"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="21"/>
+      <c r="J15" s="21"/>
+      <c r="K15" s="22"/>
+      <c r="L15" s="20"/>
+      <c r="M15" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="N15" s="21"/>
+      <c r="O15" s="22"/>
+      <c r="P15" s="20"/>
+      <c r="Q15" s="21"/>
+      <c r="R15" s="21"/>
+      <c r="S15" s="22"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" s="34" t="s">
+      <c r="A16" s="29" t="s">
         <v>25</v>
       </c>
       <c r="B16" s="7"/>
       <c r="C16" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="25"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="27"/>
-      <c r="H16" s="25"/>
-      <c r="I16" s="26"/>
-      <c r="J16" s="26"/>
-      <c r="K16" s="27"/>
-      <c r="L16" s="25"/>
-      <c r="M16" s="26"/>
-      <c r="N16" s="26"/>
-      <c r="O16" s="27"/>
-      <c r="P16" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q16" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="R16" s="26"/>
-      <c r="S16" s="27"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="21"/>
+      <c r="J16" s="21"/>
+      <c r="K16" s="22"/>
+      <c r="L16" s="20"/>
+      <c r="M16" s="21"/>
+      <c r="N16" s="21"/>
+      <c r="O16" s="22"/>
+      <c r="P16" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q16" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="R16" s="21"/>
+      <c r="S16" s="22"/>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A17" s="34" t="s">
+      <c r="A17" s="29" t="s">
         <v>26</v>
       </c>
       <c r="B17" s="7"/>
       <c r="C17" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D17" s="25"/>
-      <c r="E17" s="26"/>
-      <c r="F17" s="26"/>
-      <c r="G17" s="27"/>
-      <c r="H17" s="25"/>
-      <c r="I17" s="26"/>
-      <c r="J17" s="26"/>
-      <c r="K17" s="27"/>
-      <c r="L17" s="25"/>
-      <c r="M17" s="26"/>
-      <c r="N17" s="26"/>
-      <c r="O17" s="27"/>
-      <c r="P17" s="25"/>
-      <c r="Q17" s="26"/>
-      <c r="R17" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="S17" s="27"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="21"/>
+      <c r="J17" s="21"/>
+      <c r="K17" s="22"/>
+      <c r="L17" s="20"/>
+      <c r="M17" s="21"/>
+      <c r="N17" s="21"/>
+      <c r="O17" s="22"/>
+      <c r="P17" s="20"/>
+      <c r="Q17" s="21"/>
+      <c r="R17" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="S17" s="22"/>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A18" s="34" t="s">
+      <c r="A18" s="29" t="s">
         <v>23</v>
       </c>
       <c r="B18" s="7"/>
       <c r="C18" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D18" s="25"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="27"/>
-      <c r="H18" s="25"/>
-      <c r="I18" s="26"/>
-      <c r="J18" s="26"/>
-      <c r="K18" s="27"/>
-      <c r="L18" s="25"/>
-      <c r="M18" s="26"/>
-      <c r="N18" s="26"/>
-      <c r="O18" s="27"/>
-      <c r="P18" s="25"/>
-      <c r="Q18" s="26"/>
-      <c r="R18" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="S18" s="27"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="21"/>
+      <c r="J18" s="21"/>
+      <c r="K18" s="22"/>
+      <c r="L18" s="20"/>
+      <c r="M18" s="21"/>
+      <c r="N18" s="21"/>
+      <c r="O18" s="22"/>
+      <c r="P18" s="20"/>
+      <c r="Q18" s="21"/>
+      <c r="R18" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="S18" s="22"/>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
@@ -1403,67 +1403,67 @@
       <c r="C19" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D19" s="36"/>
-      <c r="E19" s="31"/>
-      <c r="F19" s="31"/>
-      <c r="G19" s="34"/>
-      <c r="H19" s="32"/>
-      <c r="I19" s="31"/>
-      <c r="J19" s="31"/>
-      <c r="K19" s="34"/>
-      <c r="L19" s="32"/>
-      <c r="M19" s="31"/>
-      <c r="N19" s="31"/>
+      <c r="D19" s="31"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="26"/>
+      <c r="G19" s="29"/>
+      <c r="H19" s="27"/>
+      <c r="I19" s="26"/>
+      <c r="J19" s="26"/>
+      <c r="K19" s="29"/>
+      <c r="L19" s="27"/>
+      <c r="M19" s="26"/>
+      <c r="N19" s="26"/>
       <c r="O19" s="2"/>
-      <c r="P19" s="36"/>
-      <c r="Q19" s="31"/>
-      <c r="R19" s="31"/>
-      <c r="S19" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="T19" s="38"/>
+      <c r="P19" s="31"/>
+      <c r="Q19" s="26"/>
+      <c r="R19" s="26"/>
+      <c r="S19" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="T19" s="33"/>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A20" s="23"/>
-      <c r="B20" s="35"/>
-      <c r="C20" s="23"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="23"/>
-      <c r="F20" s="23"/>
-      <c r="G20" s="23"/>
-      <c r="H20" s="23"/>
-      <c r="I20" s="23"/>
-      <c r="J20" s="23"/>
-      <c r="K20" s="23"/>
-      <c r="L20" s="23"/>
-      <c r="M20" s="23"/>
-      <c r="N20" s="23"/>
-      <c r="O20" s="23"/>
-      <c r="P20" s="23"/>
-      <c r="Q20" s="23"/>
-      <c r="R20" s="23"/>
-      <c r="S20" s="23"/>
+      <c r="A20" s="18"/>
+      <c r="B20" s="30"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="18"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
+      <c r="K20" s="18"/>
+      <c r="L20" s="18"/>
+      <c r="M20" s="18"/>
+      <c r="N20" s="18"/>
+      <c r="O20" s="18"/>
+      <c r="P20" s="18"/>
+      <c r="Q20" s="18"/>
+      <c r="R20" s="18"/>
+      <c r="S20" s="18"/>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A21" s="23"/>
-      <c r="B21" s="39"/>
-      <c r="C21" s="23"/>
-      <c r="D21" s="23"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="23"/>
-      <c r="G21" s="23"/>
-      <c r="H21" s="23"/>
-      <c r="I21" s="23"/>
-      <c r="J21" s="23"/>
-      <c r="K21" s="23"/>
-      <c r="L21" s="23"/>
-      <c r="M21" s="23"/>
-      <c r="N21" s="23"/>
-      <c r="O21" s="23"/>
-      <c r="P21" s="23"/>
-      <c r="Q21" s="23"/>
-      <c r="R21" s="23"/>
-      <c r="S21" s="23"/>
+      <c r="A21" s="18"/>
+      <c r="B21" s="34"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18"/>
+      <c r="I21" s="18"/>
+      <c r="J21" s="18"/>
+      <c r="K21" s="18"/>
+      <c r="L21" s="18"/>
+      <c r="M21" s="18"/>
+      <c r="N21" s="18"/>
+      <c r="O21" s="18"/>
+      <c r="P21" s="18"/>
+      <c r="Q21" s="18"/>
+      <c r="R21" s="18"/>
+      <c r="S21" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>